<commit_message>
Agregado de campo SoloMedidas a la cadena de custodia
</commit_message>
<xml_diff>
--- a/back/assets/CadenaCustodiaNuevo.xlsx
+++ b/back/assets/CadenaCustodiaNuevo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Netrona\BfU\ProcesoProtocolos\ModeloCadena\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a4cc160f71f82d48/Documentos/NETRONA/proyectos/BFU-ProtocolManager/back/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E372BF-BB79-4884-B1C9-21915ACE3593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{73E372BF-BB79-4884-B1C9-21915ACE3593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F9BF073-7651-48C3-B7F3-2E1265577B78}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6A2FE455-2356-4315-A54C-132DE19BA626}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{6A2FE455-2356-4315-A54C-132DE19BA626}"/>
   </bookViews>
   <sheets>
     <sheet name="CadenaCustodia" sheetId="2" r:id="rId1"/>
@@ -844,7 +844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -899,6 +899,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -908,71 +959,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1362,25 +1368,25 @@
   </sheetPr>
   <dimension ref="B1:AB38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:AB30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" customWidth="1"/>
-    <col min="2" max="5" width="4.77734375" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="8" width="4.77734375" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" customWidth="1"/>
-    <col min="10" max="13" width="4.77734375" customWidth="1"/>
-    <col min="14" max="14" width="8.77734375" customWidth="1"/>
-    <col min="15" max="18" width="4.77734375" customWidth="1"/>
-    <col min="19" max="28" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="1.86328125" customWidth="1"/>
+    <col min="2" max="5" width="4.796875" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" customWidth="1"/>
+    <col min="7" max="8" width="4.796875" customWidth="1"/>
+    <col min="9" max="9" width="8.796875" customWidth="1"/>
+    <col min="10" max="13" width="4.796875" customWidth="1"/>
+    <col min="14" max="14" width="8.796875" customWidth="1"/>
+    <col min="15" max="18" width="4.796875" customWidth="1"/>
+    <col min="19" max="28" width="8.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1391,16 +1397,16 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
-      <c r="L2" s="60" t="s">
+      <c r="L2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="60"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
@@ -1413,7 +1419,7 @@
       <c r="AA2" s="15"/>
       <c r="AB2" s="16"/>
     </row>
-    <row r="3" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="10"/>
       <c r="F3" s="11"/>
       <c r="G3" s="12"/>
@@ -1421,14 +1427,14 @@
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
       <c r="T3" s="13"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
@@ -1441,7 +1447,7 @@
       <c r="AA3" s="13"/>
       <c r="AB3" s="14"/>
     </row>
-    <row r="4" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="10"/>
       <c r="F4" s="11"/>
       <c r="G4" s="22" t="s">
@@ -1475,7 +1481,7 @@
       <c r="AA4" s="15"/>
       <c r="AB4" s="16"/>
     </row>
-    <row r="5" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="10"/>
       <c r="F5" s="11"/>
       <c r="G5" s="18" t="s">
@@ -1505,7 +1511,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="20"/>
     </row>
-    <row r="6" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="10"/>
       <c r="F6" s="11"/>
       <c r="G6" s="18" t="s">
@@ -1537,7 +1543,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="20"/>
     </row>
-    <row r="7" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="10"/>
       <c r="F7" s="11"/>
       <c r="G7" s="21" t="s">
@@ -1571,7 +1577,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="20"/>
     </row>
-    <row r="8" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="10"/>
       <c r="F8" s="11"/>
       <c r="G8" s="10" t="s">
@@ -1583,7 +1589,7 @@
       <c r="U8" s="6"/>
       <c r="AB8" s="11"/>
     </row>
-    <row r="9" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B9" s="24"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
@@ -1591,7 +1597,7 @@
       <c r="F9" s="25"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="70" t="s">
         <v>14</v>
       </c>
       <c r="J9" s="28"/>
@@ -1608,7 +1614,7 @@
       <c r="U9" s="25"/>
       <c r="V9" s="26"/>
       <c r="W9" s="25"/>
-      <c r="X9" s="28" t="s">
+      <c r="X9" s="70" t="s">
         <v>15</v>
       </c>
       <c r="Y9" s="25"/>
@@ -1616,36 +1622,36 @@
       <c r="AA9" s="25"/>
       <c r="AB9" s="26"/>
     </row>
-    <row r="10" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="63" t="s">
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="55" t="s">
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="68"/>
-      <c r="O10" s="55" t="s">
+      <c r="N10" s="52"/>
+      <c r="O10" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="P10" s="68"/>
-      <c r="Q10" s="55" t="s">
+      <c r="P10" s="52"/>
+      <c r="Q10" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="R10" s="68"/>
+      <c r="R10" s="52"/>
       <c r="S10" s="32" t="s">
         <v>27</v>
       </c>
@@ -1658,18 +1664,18 @@
       <c r="V10" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="W10" s="66" t="s">
+      <c r="W10" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="X10" s="67"/>
-      <c r="Y10" s="67"/>
-      <c r="Z10" s="68"/>
-      <c r="AA10" s="55" t="s">
+      <c r="X10" s="51"/>
+      <c r="Y10" s="51"/>
+      <c r="Z10" s="52"/>
+      <c r="AA10" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="AB10" s="56"/>
-    </row>
-    <row r="11" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB10" s="54"/>
+    </row>
+    <row r="11" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="30"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1698,7 +1704,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="30"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1727,7 +1733,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="20"/>
     </row>
-    <row r="13" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="30"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1756,7 +1762,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="30"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1785,7 +1791,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="30"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1814,7 +1820,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="30"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1843,7 +1849,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="20"/>
     </row>
-    <row r="17" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="30"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1872,7 +1878,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="20"/>
     </row>
-    <row r="18" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="30"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1901,7 +1907,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="30"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1930,7 +1936,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="30"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1959,7 +1965,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="20"/>
     </row>
-    <row r="21" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="30"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1988,7 +1994,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="30"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2017,7 +2023,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="20"/>
     </row>
-    <row r="23" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="30"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2046,7 +2052,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="30"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2075,7 +2081,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="30"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2104,7 +2110,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="30"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2133,7 +2139,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="36"/>
@@ -2162,40 +2168,40 @@
       <c r="AA27" s="36"/>
       <c r="AB27" s="40"/>
     </row>
-    <row r="28" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="47" t="s">
+    <row r="28" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
-      <c r="O28" s="48"/>
-      <c r="P28" s="48"/>
-      <c r="Q28" s="48"/>
-      <c r="R28" s="48"/>
-      <c r="S28" s="48"/>
-      <c r="T28" s="48"/>
-      <c r="U28" s="48"/>
-      <c r="V28" s="49"/>
-      <c r="W28" s="57" t="s">
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="66"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="66"/>
+      <c r="S28" s="66"/>
+      <c r="T28" s="66"/>
+      <c r="U28" s="66"/>
+      <c r="V28" s="67"/>
+      <c r="W28" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="X28" s="48"/>
-      <c r="Y28" s="48"/>
-      <c r="Z28" s="48"/>
-      <c r="AA28" s="48"/>
-      <c r="AB28" s="49"/>
-    </row>
-    <row r="29" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="X28" s="66"/>
+      <c r="Y28" s="66"/>
+      <c r="Z28" s="66"/>
+      <c r="AA28" s="66"/>
+      <c r="AB28" s="67"/>
+    </row>
+    <row r="29" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B29" s="41" t="s">
         <v>33</v>
       </c>
@@ -2230,95 +2236,95 @@
       <c r="AA29" s="36"/>
       <c r="AB29" s="40"/>
     </row>
-    <row r="30" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="47" t="s">
+    <row r="30" spans="2:28" s="68" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="48"/>
-      <c r="S30" s="48"/>
-      <c r="T30" s="48"/>
-      <c r="U30" s="48"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="48"/>
-      <c r="Z30" s="48"/>
-      <c r="AA30" s="48"/>
-      <c r="AB30" s="49"/>
-    </row>
-    <row r="31" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="54" t="s">
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="66"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="66"/>
+      <c r="O30" s="66"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="66"/>
+      <c r="S30" s="66"/>
+      <c r="T30" s="66"/>
+      <c r="U30" s="66"/>
+      <c r="V30" s="66"/>
+      <c r="W30" s="66"/>
+      <c r="X30" s="66"/>
+      <c r="Y30" s="66"/>
+      <c r="Z30" s="66"/>
+      <c r="AA30" s="66"/>
+      <c r="AB30" s="67"/>
+    </row>
+    <row r="31" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="52" t="s">
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="53"/>
-      <c r="O31" s="52" t="s">
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="50"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="50"/>
-      <c r="T31" s="53"/>
-      <c r="U31" s="52" t="s">
+      <c r="P31" s="59"/>
+      <c r="Q31" s="59"/>
+      <c r="R31" s="59"/>
+      <c r="S31" s="59"/>
+      <c r="T31" s="56"/>
+      <c r="U31" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="V31" s="50"/>
-      <c r="W31" s="50"/>
-      <c r="X31" s="53"/>
-      <c r="Y31" s="52" t="s">
+      <c r="V31" s="59"/>
+      <c r="W31" s="59"/>
+      <c r="X31" s="56"/>
+      <c r="Y31" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="Z31" s="53"/>
-      <c r="AA31" s="58" t="s">
+      <c r="Z31" s="56"/>
+      <c r="AA31" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="AB31" s="59"/>
-    </row>
-    <row r="32" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="44" t="s">
+      <c r="AB31" s="58"/>
+    </row>
+    <row r="32" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="46"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="63"/>
       <c r="N32" s="6"/>
       <c r="T32" s="6"/>
       <c r="X32" s="6"/>
       <c r="Z32" s="6"/>
       <c r="AB32" s="11"/>
     </row>
-    <row r="33" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2347,81 +2353,81 @@
       <c r="AA33" s="13"/>
       <c r="AB33" s="14"/>
     </row>
-    <row r="34" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="47" t="s">
+    <row r="34" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
-      <c r="P34" s="48"/>
-      <c r="Q34" s="48"/>
-      <c r="R34" s="48"/>
-      <c r="S34" s="48"/>
-      <c r="T34" s="48"/>
-      <c r="U34" s="48"/>
-      <c r="V34" s="48"/>
-      <c r="W34" s="48"/>
-      <c r="X34" s="48"/>
-      <c r="Y34" s="48"/>
-      <c r="Z34" s="48"/>
-      <c r="AA34" s="48"/>
-      <c r="AB34" s="49"/>
-    </row>
-    <row r="35" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="54" t="s">
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="66"/>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="66"/>
+      <c r="S34" s="66"/>
+      <c r="T34" s="66"/>
+      <c r="U34" s="66"/>
+      <c r="V34" s="66"/>
+      <c r="W34" s="66"/>
+      <c r="X34" s="66"/>
+      <c r="Y34" s="66"/>
+      <c r="Z34" s="66"/>
+      <c r="AA34" s="66"/>
+      <c r="AB34" s="67"/>
+    </row>
+    <row r="35" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="52" t="s">
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="52" t="s">
+      <c r="I35" s="59"/>
+      <c r="J35" s="59"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="M35" s="50"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="50"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="52" t="s">
+      <c r="M35" s="59"/>
+      <c r="N35" s="59"/>
+      <c r="O35" s="59"/>
+      <c r="P35" s="59"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="S35" s="50"/>
-      <c r="T35" s="53"/>
+      <c r="S35" s="59"/>
+      <c r="T35" s="56"/>
       <c r="U35" s="43" t="s">
         <v>41</v>
       </c>
       <c r="V35" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="W35" s="50" t="s">
+      <c r="W35" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="X35" s="50"/>
-      <c r="Y35" s="50"/>
-      <c r="Z35" s="50"/>
-      <c r="AA35" s="50"/>
-      <c r="AB35" s="51"/>
-    </row>
-    <row r="36" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="X35" s="59"/>
+      <c r="Y35" s="59"/>
+      <c r="Z35" s="59"/>
+      <c r="AA35" s="59"/>
+      <c r="AB35" s="64"/>
+    </row>
+    <row r="36" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B36" s="12"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
@@ -2450,13 +2456,13 @@
       <c r="AA36" s="13"/>
       <c r="AB36" s="14"/>
     </row>
-    <row r="37" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AB37" s="11"/>
     </row>
-    <row r="38" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B38" s="12"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
@@ -2489,13 +2495,13 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="L2:S3"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="W10:Z10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B34:AB34"/>
+    <mergeCell ref="W35:AB35"/>
+    <mergeCell ref="R35:T35"/>
+    <mergeCell ref="L35:Q35"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="B35:G35"/>
     <mergeCell ref="AA10:AB10"/>
     <mergeCell ref="B28:V28"/>
     <mergeCell ref="W28:AB28"/>
@@ -2506,13 +2512,13 @@
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="O31:T31"/>
     <mergeCell ref="U31:X31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B34:AB34"/>
-    <mergeCell ref="W35:AB35"/>
-    <mergeCell ref="R35:T35"/>
-    <mergeCell ref="L35:Q35"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="L2:S3"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="W10:Z10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0.11811023622047245" footer="0.11811023622047245"/>
   <pageSetup scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>